<commit_message>
1) NB Reporting: - Capital calls exporting - Comments for adjusted redemptions (Singularity GL form)
2) PE
- M2S2 memo adjustments
- Firm and Fund profile
</commit_message>
<xml_diff>
--- a/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/capital_call/CC_OA_SPV_TEMPLATE.xlsx
+++ b/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/capital_call/CC_OA_SPV_TEMPLATE.xlsx
@@ -105,9 +105,6 @@
     <t xml:space="preserve">                                                                       Date                    </t>
   </si>
   <si>
-    <t>Additional subscription</t>
-  </si>
-  <si>
     <t>Cash disbursement</t>
   </si>
   <si>
@@ -132,9 +129,6 @@
     </r>
   </si>
   <si>
-    <t>Akylzhan Baimagambetov-Director</t>
-  </si>
-  <si>
     <t>Визы:</t>
   </si>
   <si>
@@ -153,18 +147,6 @@
     <t>Исп.: Илимесова Л.К., тел.: 244 94 04 (154)</t>
   </si>
   <si>
-    <t>Рысбеков С.Д._____________</t>
-  </si>
-  <si>
-    <t>Омаров Т.М.______________</t>
-  </si>
-  <si>
-    <t>Саенко А.И._______________</t>
-  </si>
-  <si>
-    <t>Исп: Илимесова Л.К.,тел:244 94 04 (154)</t>
-  </si>
-  <si>
     <t>&lt;dd.MM.yyyy&gt;</t>
   </si>
   <si>
@@ -190,6 +172,24 @@
   </si>
   <si>
     <t>&lt;reference&gt;</t>
+  </si>
+  <si>
+    <t>&lt;investment_category&gt;</t>
+  </si>
+  <si>
+    <t>&lt;DIRECTORNAME&gt;-Director</t>
+  </si>
+  <si>
+    <t>&lt;viza_1&gt;</t>
+  </si>
+  <si>
+    <t>&lt;viza_2&gt;</t>
+  </si>
+  <si>
+    <t>&lt;doer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;viza_3&gt;</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -419,9 +419,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -460,6 +457,11 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -773,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F89"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -790,20 +792,20 @@
   <sheetData>
     <row r="1" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="26"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="27"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="3" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="22"/>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="28"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="27"/>
     </row>
     <row r="4" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
@@ -811,8 +813,8 @@
         <v>1</v>
       </c>
       <c r="D4" s="5"/>
-      <c r="E4" s="6" t="s">
-        <v>27</v>
+      <c r="E4" s="39" t="s">
+        <v>44</v>
       </c>
       <c r="F4" s="4"/>
     </row>
@@ -823,7 +825,7 @@
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" s="4"/>
     </row>
@@ -833,8 +835,8 @@
         <v>19</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="E6" s="31" t="s">
-        <v>41</v>
+      <c r="E6" s="30" t="s">
+        <v>35</v>
       </c>
       <c r="F6" s="4"/>
     </row>
@@ -844,8 +846,8 @@
         <v>20</v>
       </c>
       <c r="D7" s="5"/>
-      <c r="E7" s="32" t="s">
-        <v>42</v>
+      <c r="E7" s="31" t="s">
+        <v>36</v>
       </c>
       <c r="F7" s="4"/>
     </row>
@@ -873,8 +875,8 @@
         <v>3</v>
       </c>
       <c r="D10" s="9"/>
-      <c r="E10" s="33" t="s">
-        <v>43</v>
+      <c r="E10" s="32" t="s">
+        <v>37</v>
       </c>
       <c r="F10" s="4"/>
     </row>
@@ -884,7 +886,7 @@
         <v>6</v>
       </c>
       <c r="D11" s="9"/>
-      <c r="E11" s="30">
+      <c r="E11" s="29">
         <v>8901296082</v>
       </c>
       <c r="F11" s="4"/>
@@ -917,8 +919,8 @@
         <v>17</v>
       </c>
       <c r="D14" s="9"/>
-      <c r="E14" s="34" t="s">
-        <v>44</v>
+      <c r="E14" s="33" t="s">
+        <v>38</v>
       </c>
       <c r="F14" s="4"/>
     </row>
@@ -937,8 +939,8 @@
         <v>5</v>
       </c>
       <c r="D16" s="9"/>
-      <c r="E16" s="35" t="s">
-        <v>45</v>
+      <c r="E16" s="34" t="s">
+        <v>39</v>
       </c>
       <c r="F16" s="4"/>
     </row>
@@ -948,8 +950,8 @@
         <v>8</v>
       </c>
       <c r="D17" s="9"/>
-      <c r="E17" s="36" t="s">
-        <v>46</v>
+      <c r="E17" s="35" t="s">
+        <v>40</v>
       </c>
       <c r="F17" s="4"/>
     </row>
@@ -982,7 +984,7 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="24" t="s">
         <v>10</v>
       </c>
       <c r="D21" s="13"/>
@@ -995,8 +997,8 @@
         <v>11</v>
       </c>
       <c r="D22" s="9"/>
-      <c r="E22" s="37" t="s">
-        <v>47</v>
+      <c r="E22" s="36" t="s">
+        <v>41</v>
       </c>
       <c r="F22" s="4"/>
     </row>
@@ -1006,8 +1008,8 @@
         <v>12</v>
       </c>
       <c r="D23" s="9"/>
-      <c r="E23" s="38" t="s">
-        <v>48</v>
+      <c r="E23" s="37" t="s">
+        <v>42</v>
       </c>
       <c r="F23" s="4"/>
     </row>
@@ -1036,7 +1038,7 @@
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="11" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F26" s="4"/>
     </row>
@@ -1074,19 +1076,19 @@
     </row>
     <row r="31" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="2"/>
-      <c r="C31" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" s="24"/>
-      <c r="E31" s="39" t="s">
-        <v>41</v>
+      <c r="C31" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="23"/>
+      <c r="E31" s="38" t="s">
+        <v>35</v>
       </c>
       <c r="F31" s="4"/>
     </row>
     <row r="32" spans="2:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="2"/>
       <c r="C32" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D32" s="21"/>
       <c r="E32" s="8" t="s">
@@ -1102,72 +1104,72 @@
       <c r="F33" s="8"/>
     </row>
     <row r="78" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C78" s="29" t="s">
+      <c r="C78" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D78" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="E78" s="28"/>
+    </row>
+    <row r="79" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C79" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="D79" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E79" s="28"/>
+    </row>
+    <row r="80" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C80" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D80" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="D78" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="E78" s="29"/>
-    </row>
-    <row r="79" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C79" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="D79" s="29" t="s">
+      <c r="E80" s="28"/>
+    </row>
+    <row r="81" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C81" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="D81" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="E79" s="29"/>
-    </row>
-    <row r="80" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C80" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="D80" s="29" t="s">
+      <c r="E81" s="28"/>
+    </row>
+    <row r="82" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C82" s="28"/>
+      <c r="D82" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="E80" s="29"/>
-    </row>
-    <row r="81" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C81" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D81" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="E81" s="29"/>
-    </row>
-    <row r="82" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C82" s="29"/>
-      <c r="D82" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="E82" s="29"/>
+      <c r="E82" s="28"/>
     </row>
     <row r="83" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C83" s="29"/>
-      <c r="D83" s="29"/>
-      <c r="E83" s="29"/>
+      <c r="C83" s="28"/>
+      <c r="D83" s="28"/>
+      <c r="E83" s="28"/>
     </row>
     <row r="84" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C84" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="D84" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="E84" s="29"/>
+      <c r="C84" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="D84" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E84" s="28"/>
     </row>
     <row r="85" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C85" s="29"/>
-      <c r="D85" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="E85" s="29"/>
+      <c r="C85" s="28"/>
+      <c r="D85" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E85" s="28"/>
     </row>
     <row r="89" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D89" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>